<commit_message>
Added verb roots to evolver
</commit_message>
<xml_diff>
--- a/new docs/inflections.xlsx
+++ b/new docs/inflections.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_langa\redlang\Proto-Azxish\new docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFEF46B-B69C-4BAD-B5C5-1F50402D907A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C22B215-A556-4080-864A-7712DB8CC025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{45993D0C-CED6-407A-B4F5-5E017F34C1EA}"/>
+    <workbookView xWindow="16896" yWindow="2448" windowWidth="11748" windowHeight="12360" xr2:uid="{45993D0C-CED6-407A-B4F5-5E017F34C1EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Verbs" sheetId="1" r:id="rId1"/>
+    <sheet name="Verbs (Updated)" sheetId="2" r:id="rId1"/>
+    <sheet name="Verbs (Old)" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="363">
   <si>
     <t>English</t>
   </si>
@@ -2508,6 +2509,471 @@
   </si>
   <si>
     <t>/ˈħæo̯̯ʋɛʋæˌɕæɲ̊cɛf/</t>
+  </si>
+  <si>
+    <t>uqñî</t>
+  </si>
+  <si>
+    <t>To hold / To grab</t>
+  </si>
+  <si>
+    <t>To swell / To be swollen</t>
+  </si>
+  <si>
+    <t>qéśśwèñañ</t>
+  </si>
+  <si>
+    <t>qilîhaq</t>
+  </si>
+  <si>
+    <t>ˈɢeɕˌɕɣɛɴæɴ̥</t>
+  </si>
+  <si>
+    <t>qúnhíññi</t>
+  </si>
+  <si>
+    <t>ˈɢun̥ˌħiɴ̥ɴ̥i</t>
+  </si>
+  <si>
+    <t>utwiqñî</t>
+  </si>
+  <si>
+    <t>qêjuqñî</t>
+  </si>
+  <si>
+    <t>mêwuqñî</t>
+  </si>
+  <si>
+    <t>âvuqñî</t>
+  </si>
+  <si>
+    <t>mîtuqñî</t>
+  </si>
+  <si>
+    <t>huqêjuqñî</t>
+  </si>
+  <si>
+    <t>hûmêwuqñî</t>
+  </si>
+  <si>
+    <t>hevâvuqñî</t>
+  </si>
+  <si>
+    <t>hefmîtuqñî</t>
+  </si>
+  <si>
+    <t>lîhaq &gt; ˈljɐ̃æq̚</t>
+  </si>
+  <si>
+    <t>úioñaʔ</t>
+  </si>
+  <si>
+    <t>ˈuɪ̯ɔɴæʔ</t>
+  </si>
+  <si>
+    <t>qúʔñə</t>
+  </si>
+  <si>
+    <t>ˈɢuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>qúiúʔñə</t>
+  </si>
+  <si>
+    <t>ˈɢuɪ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>ˈmyˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>mýúʔñə</t>
+  </si>
+  <si>
+    <t>qáuúʔñə</t>
+  </si>
+  <si>
+    <t>ˈɢɑʊ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>ˈmiˌduʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>mídúʔñə</t>
+  </si>
+  <si>
+    <t>ˈħuɢɢuɪ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>húqquiúʔñə</t>
+  </si>
+  <si>
+    <t>húomouúʔñə</t>
+  </si>
+  <si>
+    <t>ˈħuo̯mou̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>hóuvâuúʔñə</t>
+  </si>
+  <si>
+    <t>ˈħou̯ʋɑʊ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>ˈħɑʊ̯mɤˌtuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>háumətúʔñə</t>
+  </si>
+  <si>
+    <t>êqjuqñî</t>
+  </si>
+  <si>
+    <t>jéñwúʔñə</t>
+  </si>
+  <si>
+    <t>ˈjeɴˌɣuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>twimêwuqñî</t>
+  </si>
+  <si>
+    <t>âxâvuqñî</t>
+  </si>
+  <si>
+    <t>îmîtuqñî</t>
+  </si>
+  <si>
+    <t>ˈtħim̥pøʊ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>thímpøuúʔñə</t>
+  </si>
+  <si>
+    <t>ˈɢʌr̥ɑʊ̯ˌuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>qářâuúʔñə</t>
+  </si>
+  <si>
+    <t>ˈɟie̯ɲiˌtuʔɴ̥ɤ</t>
+  </si>
+  <si>
+    <t>ǵíeńitúʔñə</t>
+  </si>
+  <si>
+    <t>qêlîhaqkan</t>
+  </si>
+  <si>
+    <t>mûlîhaqkan</t>
+  </si>
+  <si>
+    <t>vâlîhaqkan</t>
+  </si>
+  <si>
+    <t>mîlîhaqkan</t>
+  </si>
+  <si>
+    <t>huqêlîhaqkan</t>
+  </si>
+  <si>
+    <t>hûmûlîhaqkan</t>
+  </si>
+  <si>
+    <t>hefmîlîhaqkan</t>
+  </si>
+  <si>
+    <t>êqlîhaqkan</t>
+  </si>
+  <si>
+    <t>twimûlîhaqkan</t>
+  </si>
+  <si>
+    <t>xâvâlîhaqkan</t>
+  </si>
+  <si>
+    <t>îmîlîhaqkan</t>
+  </si>
+  <si>
+    <t>qǿihàań</t>
+  </si>
+  <si>
+    <t>ˈɢøiˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>múľəhàań</t>
+  </si>
+  <si>
+    <t>ˈmuʎɤˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>váuəhàań</t>
+  </si>
+  <si>
+    <t>ˈʋɑʊ̯ɤˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>ˈmymiˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>mýmihàań</t>
+  </si>
+  <si>
+    <t>húqqouəhàań</t>
+  </si>
+  <si>
+    <t>ˈħuɢɢou̯ɤˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>ˈħuo̯muʎɤˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>húomuľəhàań</t>
+  </si>
+  <si>
+    <t>qêjuqñîke</t>
+  </si>
+  <si>
+    <t>qéiyʔñíñe</t>
+  </si>
+  <si>
+    <t>mêwuqñîke</t>
+  </si>
+  <si>
+    <t>mýyʔñíñe</t>
+  </si>
+  <si>
+    <t>âvuqñîke</t>
+  </si>
+  <si>
+    <t>mîtuqñîke</t>
+  </si>
+  <si>
+    <t>mínyʔñíñe</t>
+  </si>
+  <si>
+    <t>êqjuqñîke</t>
+  </si>
+  <si>
+    <t>twimêwuqñîke</t>
+  </si>
+  <si>
+    <t>âxâvuqñîke</t>
+  </si>
+  <si>
+    <t>îmîtuqñîke</t>
+  </si>
+  <si>
+    <t>huqêjuqñîke</t>
+  </si>
+  <si>
+    <t>húqquiuʔñíñe</t>
+  </si>
+  <si>
+    <t>hûmêwuqñîke</t>
+  </si>
+  <si>
+    <t>húomouuʔñíñe</t>
+  </si>
+  <si>
+    <t>hevâvuqñîke</t>
+  </si>
+  <si>
+    <t>hefmîtuqñîke</t>
+  </si>
+  <si>
+    <t>hǿumityʔñíñe</t>
+  </si>
+  <si>
+    <t>qáuuʔñíñe</t>
+  </si>
+  <si>
+    <t>hǿuvâuyʔñíñe</t>
+  </si>
+  <si>
+    <t>ˈɢei̯yʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈmyyʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈɢɑʊ̯uʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈminyʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈħuɢɢuɪ̯uʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈħuo̯mou̯uʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈħøʊ̯ʋɑʊ̯yʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ˈħøʊ̯mityʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>qêlîhaqknef</t>
+  </si>
+  <si>
+    <t>qǿihàńef</t>
+  </si>
+  <si>
+    <t>mûlîhaqknef</t>
+  </si>
+  <si>
+    <t>múľəhàńef</t>
+  </si>
+  <si>
+    <t>vâlîhaqknef</t>
+  </si>
+  <si>
+    <t>váuəhàńef</t>
+  </si>
+  <si>
+    <t>mîlîhaqknef</t>
+  </si>
+  <si>
+    <t>mýmihàńef</t>
+  </si>
+  <si>
+    <t>êqlîhaqknef</t>
+  </si>
+  <si>
+    <t>jéñeľihàńef</t>
+  </si>
+  <si>
+    <t>twimûlîhaqknef</t>
+  </si>
+  <si>
+    <t>thímpyľihàńef</t>
+  </si>
+  <si>
+    <t>xâvâlîhaqknef</t>
+  </si>
+  <si>
+    <t>âřřáuâuəhàńef</t>
+  </si>
+  <si>
+    <t>îmîlîhaqknef</t>
+  </si>
+  <si>
+    <t>ǵíeńyihàńef</t>
+  </si>
+  <si>
+    <t>huqêlîhaqknef</t>
+  </si>
+  <si>
+    <t>húqqouəhàńef</t>
+  </si>
+  <si>
+    <t>hûmûlîhaqknef</t>
+  </si>
+  <si>
+    <t>húomuľəhàńef</t>
+  </si>
+  <si>
+    <t>hâvelîhaqknef</t>
+  </si>
+  <si>
+    <t>háuâuľəhàńef</t>
+  </si>
+  <si>
+    <t>hefmîlîhaqknef</t>
+  </si>
+  <si>
+    <t>hǿumyihàńef</t>
+  </si>
+  <si>
+    <t>ˈɢøiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈmuʎɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈʋɑʊ̯ɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈmymiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈjeɴɛʎiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈtħim̥pyʎiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ʌr̥ˈr̥ɑʊ̯ɑʊ̯ɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈɟie̯ɲyiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈħuɢɢou̯ɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈħuo̯muʎɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈħɑʊ̯ɑʊ̯ʎɤˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>ˈħøʊ̯myiˌħæɲ̊ɛf</t>
+  </si>
+  <si>
+    <t>hǿumyihàań</t>
+  </si>
+  <si>
+    <t>ˈħøʊ̯myiˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>jéñeľihàań</t>
+  </si>
+  <si>
+    <t>ˈjeɴɛʎiˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>jéñwyʔñíñe</t>
+  </si>
+  <si>
+    <t>ˈjeɴɣyʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>thímpyľihàań</t>
+  </si>
+  <si>
+    <t>ˈtħim̥pyʎiˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>thímpøuyʔñíñe</t>
+  </si>
+  <si>
+    <t>ˈtħim̥pøʊ̯yʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>âřřáuâuəhàań</t>
+  </si>
+  <si>
+    <t>ʌr̥ˈr̥ɑʊ̯ɑʊ̯ɤˌħææɲ̊</t>
+  </si>
+  <si>
+    <t>qāřâuyʔñíñe</t>
+  </si>
+  <si>
+    <t>ˈɢar̥ɑʊ̯yʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ǵíeńityʔñíñe</t>
+  </si>
+  <si>
+    <t>ˈɟie̯ɲityʔˌɴ̥iɴɛ</t>
+  </si>
+  <si>
+    <t>ǵíeńyihàań</t>
+  </si>
+  <si>
+    <t>ˈɟie̯ɲyiˌħææɲ̊</t>
   </si>
 </sst>
 </file>
@@ -2668,18 +3134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -2688,9 +3148,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2700,6 +3157,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2709,11 +3171,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3027,343 +3496,1026 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABB079F-FB94-4185-BD76-246F32A07EF6}">
+  <dimension ref="A1:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10"/>
+      <c r="B1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="17"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5062BC3C-9336-42F3-8F26-7D1FFB65358C}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+      <selection pane="topRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" style="15" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10"/>
+      <c r="B1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="N1" s="8"/>
+      <c r="L1" s="14"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>113</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="30"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>114</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
+    </row>
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="25" t="s">
         <v>182</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="19" t="s">
         <v>184</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="L7" s="15"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="19" t="s">
         <v>185</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="L8" s="15"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="21" t="s">
         <v>186</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="24"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="19" t="s">
         <v>187</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="19" t="s">
         <v>188</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="L11" s="15"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="19" t="s">
         <v>202</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="L12" s="18"/>
-      <c r="M12" s="22"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -3375,101 +4527,101 @@
       <c r="E13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="19" t="s">
         <v>189</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="20" t="s">
         <v>190</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="23"/>
-    </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="L14" s="14"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="18" t="s">
+      <c r="E15" s="19"/>
+      <c r="F15" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>191</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="22"/>
-    </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="L15" s="15"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="19" t="s">
         <v>192</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="22"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -3478,230 +4630,230 @@
       <c r="D17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="21" t="s">
         <v>193</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="24"/>
-    </row>
-    <row r="18" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="L17" s="16"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>140</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>141</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>143</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="L20" s="18"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>142</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="L21" s="15"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="5" t="s">
         <v>179</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L22" s="17"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="L22" s="14"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="19" t="s">
         <v>144</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="22"/>
-    </row>
-    <row r="24" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="L23" s="15"/>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="19" t="s">
         <v>201</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="22"/>
-    </row>
-    <row r="25" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+      <c r="L24" s="15"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="16" t="s">
         <v>135</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -3710,98 +4862,98 @@
       <c r="H25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L25" s="19"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" s="7" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:14" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="5" t="s">
         <v>148</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="19" t="s">
         <v>150</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="22"/>
-    </row>
-    <row r="28" spans="1:14" s="8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="L27" s="15"/>
+      <c r="M27" s="19"/>
+    </row>
+    <row r="28" spans="1:14" s="6" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="19" t="s">
         <v>169</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="22"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:14" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="21" t="s">
         <v>168</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="16" t="s">
         <v>139</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -3810,7 +4962,7 @@
       <c r="H29" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="L29" s="19"/>
+      <c r="L29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>